<commit_message>
Added logic to program, and condensed code
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -463,7 +463,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>62000</v>
+        <v>65000</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -471,13 +471,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4030</v>
+        <v>4225</v>
       </c>
       <c r="D2" t="n">
-        <v>1690</v>
+        <v>1990</v>
       </c>
       <c r="E2" t="n">
-        <v>2340</v>
+        <v>2235</v>
       </c>
     </row>
   </sheetData>
@@ -491,7 +491,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,40 +524,70 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Electricity</t>
+          <t>Car Insurance</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>55</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Car Insurance</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>180</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Internet</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Savings</t>
         </is>
       </c>
       <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Internet</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Miscellaneous</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>300</v>
       </c>
     </row>

</xml_diff>